<commit_message>
Allow BAU Industrial CCS fractions to be specified separately for energy and process emissions (#203)
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\ccs\BFoCPAbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\ccs\BFoCPAbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEBD663-B14A-45FD-97FE-BAD87AF759F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBE8205-C7BE-40FD-8A56-2F11E6CC8F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="2850" windowWidth="25065" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Rhodium" sheetId="17" r:id="rId3"/>
     <sheet name="BAU Calculations" sheetId="14" r:id="rId4"/>
     <sheet name="BFoCPAbS-electricity" sheetId="15" r:id="rId5"/>
-    <sheet name="BFoCPAbS-industry" sheetId="16" r:id="rId6"/>
+    <sheet name="BFoCPAbS-industry-energyEmis" sheetId="16" r:id="rId6"/>
+    <sheet name="BFoCPAbS-industry-processEmis" sheetId="18" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Global CCS Database'!$A$3:$E$71</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="121">
   <si>
     <t>Notes</t>
   </si>
@@ -5777,9 +5778,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5908,8 +5907,11 @@
       <c r="C25" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{9F56C773-538A-430B-B0A2-73F11947555B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5918,7 +5920,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C4" sqref="C4:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5933,6 +5935,16 @@
         <v>74</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <f>SUM(C4,C6,C8,C10)/SUM(C4:C15)</f>
+        <v>0.70194680559363876</v>
+      </c>
+      <c r="D2" s="15">
+        <f>10/142</f>
+        <v>7.0422535211267609E-2</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>78</v>
@@ -7182,8 +7194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7352,7 +7364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB5266F-BD5E-4822-BA8F-3811C6ED8EBD}">
   <dimension ref="A1:AH141"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J43" sqref="J43:S43"/>
     </sheetView>
   </sheetViews>
@@ -13978,9 +13990,7 @@
   </sheetPr>
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15666,9 +15676,7 @@
   </sheetPr>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AF26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -19002,4 +19010,3347 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBC9F1EA-2988-4BBD-90EC-E6E6E625E19B}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:AF26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="44.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="H1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A2,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A3,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A4,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A5,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A6,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF7">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A7,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A8,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A9,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>1.4302603032887405E-2</v>
+      </c>
+      <c r="K10">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>2.8278731947973826E-2</v>
+      </c>
+      <c r="L10">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>4.2551197441092821E-2</v>
+      </c>
+      <c r="M10">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>5.7021054798192104E-2</v>
+      </c>
+      <c r="N10">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>7.092094618782388E-2</v>
+      </c>
+      <c r="O10">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>8.4867616340924421E-2</v>
+      </c>
+      <c r="P10">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.7934444837183776E-2</v>
+      </c>
+      <c r="Q10">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11155887905676573</v>
+      </c>
+      <c r="R10">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11027775042200332</v>
+      </c>
+      <c r="S10">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10921506763073048</v>
+      </c>
+      <c r="T10">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10908558214442685</v>
+      </c>
+      <c r="U10">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10815710294166468</v>
+      </c>
+      <c r="V10">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10841179763990606</v>
+      </c>
+      <c r="W10">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10802385125586667</v>
+      </c>
+      <c r="X10">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10779498743445189</v>
+      </c>
+      <c r="Y10">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10772121961190791</v>
+      </c>
+      <c r="Z10">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10722131825715822</v>
+      </c>
+      <c r="AA10">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10682428245670701</v>
+      </c>
+      <c r="AB10">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10742164242045486</v>
+      </c>
+      <c r="AC10">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10706666229227974</v>
+      </c>
+      <c r="AD10">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10672992112007014</v>
+      </c>
+      <c r="AE10">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10677382613952834</v>
+      </c>
+      <c r="AF10">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10580769668863964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>2.7214829715730898E-2</v>
+      </c>
+      <c r="C11">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>4.1861150442235852E-2</v>
+      </c>
+      <c r="D11">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>5.2772097873378832E-2</v>
+      </c>
+      <c r="E11">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>6.3289462678504924E-2</v>
+      </c>
+      <c r="F11">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>7.1619033170092022E-2</v>
+      </c>
+      <c r="G11">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>8.0248885960188268E-2</v>
+      </c>
+      <c r="H11">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>8.8744174199345494E-2</v>
+      </c>
+      <c r="I11">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11044168709690065</v>
+      </c>
+      <c r="J11">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.12977541507774237</v>
+      </c>
+      <c r="K11">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.14851741803271179</v>
+      </c>
+      <c r="L11">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16597051109094743</v>
+      </c>
+      <c r="M11">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.18250394114552934</v>
+      </c>
+      <c r="N11">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.19805128238472208</v>
+      </c>
+      <c r="O11">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.21285712465184151</v>
+      </c>
+      <c r="P11">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.22547344970332839</v>
+      </c>
+      <c r="Q11">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.23703309978689469</v>
+      </c>
+      <c r="R11">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.23010973064913401</v>
+      </c>
+      <c r="S11">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.22656075152920011</v>
+      </c>
+      <c r="T11">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.22341180962001911</v>
+      </c>
+      <c r="U11">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.22060889378337575</v>
+      </c>
+      <c r="V11">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.21796225705452099</v>
+      </c>
+      <c r="W11">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.21545696352270516</v>
+      </c>
+      <c r="X11">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.21275643621905999</v>
+      </c>
+      <c r="Y11">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.20902556556854876</v>
+      </c>
+      <c r="Z11">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.20558434359348723</v>
+      </c>
+      <c r="AA11">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.20152259911219586</v>
+      </c>
+      <c r="AB11">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.19850165477144999</v>
+      </c>
+      <c r="AC11">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.19586944635444359</v>
+      </c>
+      <c r="AD11">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.19295510334396135</v>
+      </c>
+      <c r="AE11">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.18919433415943607</v>
+      </c>
+      <c r="AF11">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.18560515904050501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF12">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A12,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF13">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A13,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>2.0505948021545795E-3</v>
+      </c>
+      <c r="D14">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>4.1902649098006679E-3</v>
+      </c>
+      <c r="E14">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>6.297555949358883E-3</v>
+      </c>
+      <c r="F14">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>8.3487805321542825E-3</v>
+      </c>
+      <c r="G14">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>1.0343695884067968E-2</v>
+      </c>
+      <c r="H14">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>1.2383516885175775E-2</v>
+      </c>
+      <c r="I14">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>1.7886074562222763E-2</v>
+      </c>
+      <c r="J14">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>3.7817673215588633E-2</v>
+      </c>
+      <c r="K14">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>5.7439054144320545E-2</v>
+      </c>
+      <c r="L14">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>7.6772707255191058E-2</v>
+      </c>
+      <c r="M14">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.5798349977348332E-2</v>
+      </c>
+      <c r="N14">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11449013918810755</v>
+      </c>
+      <c r="O14">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.13291245448900341</v>
+      </c>
+      <c r="P14">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15115904446196166</v>
+      </c>
+      <c r="Q14">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16816065619767853</v>
+      </c>
+      <c r="R14">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16605951507039143</v>
+      </c>
+      <c r="S14">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16451657685699425</v>
+      </c>
+      <c r="T14">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16300175831518043</v>
+      </c>
+      <c r="U14">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.16149512253346063</v>
+      </c>
+      <c r="V14">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15994395018043661</v>
+      </c>
+      <c r="W14">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15837994664576605</v>
+      </c>
+      <c r="X14">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15686462025565923</v>
+      </c>
+      <c r="Y14">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15538812970311827</v>
+      </c>
+      <c r="Z14">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15391636907295844</v>
+      </c>
+      <c r="AA14">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15243507083796456</v>
+      </c>
+      <c r="AB14">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.15099240634828368</v>
+      </c>
+      <c r="AC14">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.14955418913188273</v>
+      </c>
+      <c r="AD14">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.14813758729153001</v>
+      </c>
+      <c r="AE14">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.1467304085081686</v>
+      </c>
+      <c r="AF14">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A14,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.14533138913393187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A15,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A16,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A17,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A18,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A19,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A20,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A21,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF22">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A22,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF23">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A23,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.3541600812401648E-2</v>
+      </c>
+      <c r="C24">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.8867666557611047E-2</v>
+      </c>
+      <c r="D24">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10175448028799561</v>
+      </c>
+      <c r="E24">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10129073311502906</v>
+      </c>
+      <c r="F24">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.9379181355551877E-2</v>
+      </c>
+      <c r="G24">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>9.7684617292653153E-2</v>
+      </c>
+      <c r="H24">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10029041548565455</v>
+      </c>
+      <c r="I24">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10211410944978749</v>
+      </c>
+      <c r="J24">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.1047452973549975</v>
+      </c>
+      <c r="K24">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10497066617656173</v>
+      </c>
+      <c r="L24">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10558638601237019</v>
+      </c>
+      <c r="M24">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10772411625610311</v>
+      </c>
+      <c r="N24">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10965393995789599</v>
+      </c>
+      <c r="O24">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.1121247660029908</v>
+      </c>
+      <c r="P24">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11422648898702277</v>
+      </c>
+      <c r="Q24">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11634691775502909</v>
+      </c>
+      <c r="R24">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11530406267623144</v>
+      </c>
+      <c r="S24">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11317178449957704</v>
+      </c>
+      <c r="T24">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11181533280501373</v>
+      </c>
+      <c r="U24">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.11029140435618591</v>
+      </c>
+      <c r="V24">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10892421633712464</v>
+      </c>
+      <c r="W24">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10851569312121145</v>
+      </c>
+      <c r="X24">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10851338449049105</v>
+      </c>
+      <c r="Y24">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.1079695717459391</v>
+      </c>
+      <c r="Z24">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.107208902790975</v>
+      </c>
+      <c r="AA24">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10698462657401019</v>
+      </c>
+      <c r="AB24">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10735055636181939</v>
+      </c>
+      <c r="AC24">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10735449529662218</v>
+      </c>
+      <c r="AD24">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.1076469500150212</v>
+      </c>
+      <c r="AE24">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10827780241309116</v>
+      </c>
+      <c r="AF24">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A24,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0.10842115102443392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF25">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A25,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26">
+        <f>IFERROR(INDEX('BAU Calculations'!B$112:B$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <f>IFERROR(INDEX('BAU Calculations'!C$112:C$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <f>IFERROR(INDEX('BAU Calculations'!D$112:D$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <f>IFERROR(INDEX('BAU Calculations'!E$112:E$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <f>IFERROR(INDEX('BAU Calculations'!F$112:F$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <f>IFERROR(INDEX('BAU Calculations'!G$112:G$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <f>IFERROR(INDEX('BAU Calculations'!H$112:H$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB26">
+        <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC26">
+        <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF26">
+        <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A26,'BAU Calculations'!$A$112:$A$115,0)),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct error in BFoCPAbS
</commit_message>
<xml_diff>
--- a/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
+++ b/InputData/ccs/BFoCPAbS/BAU Fraction of CCS Potential Achieved by Sector.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us-analysis\InputData\ccs\BFoCPAbS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ccs\BFoCPAbS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48909B86-8426-43C9-8BC8-95AF005BC109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805DCBE1-EE3D-4DFA-AD94-141E73B46DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1385,73 +1385,73 @@
                   <c:v>5.5847753331103325E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.305660112124406E-2</c:v>
+                  <c:v>8.7064541926442349E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.9590929459826964E-2</c:v>
+                  <c:v>0.11705880094392404</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.7086053221409809E-2</c:v>
+                  <c:v>0.14851127749752255</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.4788272018669314E-2</c:v>
+                  <c:v>0.18050218542991664</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.1642526929346116E-2</c:v>
+                  <c:v>0.2106884008874772</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.8643449064837241E-2</c:v>
+                  <c:v>0.24109980506566731</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.10474738440532255</c:v>
+                  <c:v>0.26913734538202028</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.11155887905676753</c:v>
+                  <c:v>0.29881842604490821</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.11027775042200511</c:v>
+                  <c:v>0.29538683148750888</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.10921506763073226</c:v>
+                  <c:v>0.29254035972517095</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.10908558214442861</c:v>
+                  <c:v>0.29219352360114331</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.10815710294166644</c:v>
+                  <c:v>0.28970652573660183</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.10841179763990781</c:v>
+                  <c:v>0.29038874367831979</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.10802385125586841</c:v>
+                  <c:v>0.28934960157821427</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.10779498743445363</c:v>
+                  <c:v>0.28873657348513898</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.10772121961190965</c:v>
+                  <c:v>0.28853898110332477</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.10722131825715996</c:v>
+                  <c:v>0.28719995961738809</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.10682428245670875</c:v>
+                  <c:v>0.28613647086617949</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.1074216424204566</c:v>
+                  <c:v>0.28773654219764694</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.10706666229228147</c:v>
+                  <c:v>0.28678570256860642</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.10672992112007187</c:v>
+                  <c:v>0.28588371728590217</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.10677382613953007</c:v>
+                  <c:v>0.28600132001659379</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.10580769668864136</c:v>
+                  <c:v>0.28341347327314187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1619,76 +1619,76 @@
                   <c:v>2.9372461844434771E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1353109362302647E-2</c:v>
+                  <c:v>5.1353109362300677E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.9093467852570751E-2</c:v>
+                  <c:v>5.413614667720483E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10587163526180934</c:v>
+                  <c:v>5.6871469261761405E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13120047316016237</c:v>
+                  <c:v>5.9288843556340676E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.1553034029423305</c:v>
+                  <c:v>6.1542838545548761E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.17811970888717182</c:v>
+                  <c:v>6.3612441513390683E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.19987053989390122</c:v>
+                  <c:v>6.557582402523271E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.21916693670968349</c:v>
+                  <c:v>6.6996582847732231E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.23703309978689469</c:v>
+                  <c:v>6.8236801453802204E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.23010973064913401</c:v>
+                  <c:v>6.6243710338386275E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.22656075152920011</c:v>
+                  <c:v>6.5222034531132594E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.22341180962001911</c:v>
+                  <c:v>6.4315520951216856E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.22060889378337575</c:v>
+                  <c:v>6.3508620937637719E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.21796225705452099</c:v>
+                  <c:v>6.2746710364179545E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.21545696352270516</c:v>
+                  <c:v>6.2025489498959835E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.21275643621905999</c:v>
+                  <c:v>6.1248064972152905E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.20902556556854876</c:v>
+                  <c:v>6.0174026451551198E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.20558434359348723</c:v>
+                  <c:v>5.9183371640548647E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.20152259911219586</c:v>
+                  <c:v>5.8014081562601148E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.19850165477144999</c:v>
+                  <c:v>5.7144415767537954E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.19586944635444359</c:v>
+                  <c:v>5.6386658799005812E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.19295510334396135</c:v>
+                  <c:v>5.5547681265685184E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.18919433415943607</c:v>
+                  <c:v>5.4465035591352157E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.18560515904050501</c:v>
+                  <c:v>5.3431788208629594E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3283,76 +3283,76 @@
                   <c:v>6.6700000000000728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.850000000000364</c:v>
+                  <c:v>11.849999999999909</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.618749999999636</c:v>
+                  <c:v>12.743749999999864</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.387499999998909</c:v>
+                  <c:v>13.637499999999818</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32.15625</c:v>
+                  <c:v>14.531249999999773</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>38.924999999999272</c:v>
+                  <c:v>15.424999999999955</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45.693750000000364</c:v>
+                  <c:v>16.318749999999909</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>52.462499999999636</c:v>
+                  <c:v>17.212499999999864</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>59.231249999998909</c:v>
+                  <c:v>18.106249999999818</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>66</c:v>
+                  <c:v>18.999999999999773</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3925,73 +3925,73 @@
                   <c:v>13.635000000000218</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.430625000000418</c:v>
+                  <c:v>21.305624999999054</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>17.226250000000164</c:v>
+                  <c:v>28.976249999999709</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.021875000000364</c:v>
+                  <c:v>36.646874999998545</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.817500000000109</c:v>
+                  <c:v>44.3174999999992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.613125000000309</c:v>
+                  <c:v>51.988124999999854</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.408750000000509</c:v>
+                  <c:v>59.65874999999869</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>26.204375000000255</c:v>
+                  <c:v>67.329374999999345</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>28.000000000000455</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6495,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -8046,7 +8046,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
@@ -9327,8 +9327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000817FC-5CAD-42B5-92F8-1A675198574D}">
   <dimension ref="A25:H51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9393,7 +9393,8 @@
         <v>37</v>
       </c>
       <c r="B35">
-        <v>28</v>
+        <f>28+47</f>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -9401,8 +9402,8 @@
         <v>38</v>
       </c>
       <c r="B36">
-        <f>19+47</f>
-        <v>66</v>
+        <f>19</f>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -9497,7 +9498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB5266F-BD5E-4822-BA8F-3811C6ED8EBD}">
   <dimension ref="A1:AH141"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A97" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -10001,7 +10002,7 @@
       </c>
       <c r="C34" s="24">
         <f>Rhodium!B35</f>
-        <v>28</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10014,7 +10015,7 @@
       </c>
       <c r="C35" s="24">
         <f>Rhodium!B36</f>
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10194,95 +10195,95 @@
       </c>
       <c r="L40" s="15">
         <f t="shared" si="2"/>
-        <v>15.430625000000418</v>
+        <v>21.305624999999054</v>
       </c>
       <c r="M40" s="15">
         <f t="shared" si="2"/>
-        <v>17.226250000000164</v>
+        <v>28.976249999999709</v>
       </c>
       <c r="N40" s="15">
         <f t="shared" si="2"/>
-        <v>19.021875000000364</v>
+        <v>36.646874999998545</v>
       </c>
       <c r="O40" s="15">
         <f t="shared" si="2"/>
-        <v>20.817500000000109</v>
+        <v>44.3174999999992</v>
       </c>
       <c r="P40" s="15">
         <f t="shared" si="2"/>
-        <v>22.613125000000309</v>
+        <v>51.988124999999854</v>
       </c>
       <c r="Q40" s="15">
         <f t="shared" si="2"/>
-        <v>24.408750000000509</v>
+        <v>59.65874999999869</v>
       </c>
       <c r="R40" s="15">
         <f t="shared" si="2"/>
-        <v>26.204375000000255</v>
+        <v>67.329374999999345</v>
       </c>
       <c r="S40" s="15">
         <f t="shared" si="2"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="T40" s="15">
         <f t="shared" ref="T40:AH40" si="3">S40</f>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="U40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="V40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="W40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="X40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="Y40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="Z40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AA40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AB40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AC40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AD40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AE40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AF40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AG40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
       <c r="AH40" s="15">
         <f t="shared" si="3"/>
-        <v>28.000000000000455</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10327,99 +10328,99 @@
       </c>
       <c r="K41" s="15">
         <f t="shared" si="2"/>
-        <v>11.850000000000364</v>
+        <v>11.849999999999909</v>
       </c>
       <c r="L41" s="15">
         <f t="shared" si="2"/>
-        <v>18.618749999999636</v>
+        <v>12.743749999999864</v>
       </c>
       <c r="M41" s="15">
         <f t="shared" si="2"/>
-        <v>25.387499999998909</v>
+        <v>13.637499999999818</v>
       </c>
       <c r="N41" s="15">
         <f t="shared" si="2"/>
-        <v>32.15625</v>
+        <v>14.531249999999773</v>
       </c>
       <c r="O41" s="15">
         <f t="shared" si="2"/>
-        <v>38.924999999999272</v>
+        <v>15.424999999999955</v>
       </c>
       <c r="P41" s="15">
         <f t="shared" si="2"/>
-        <v>45.693750000000364</v>
+        <v>16.318749999999909</v>
       </c>
       <c r="Q41" s="15">
         <f t="shared" si="2"/>
-        <v>52.462499999999636</v>
+        <v>17.212499999999864</v>
       </c>
       <c r="R41" s="15">
         <f t="shared" si="2"/>
-        <v>59.231249999998909</v>
+        <v>18.106249999999818</v>
       </c>
       <c r="S41" s="15">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="T41" s="15">
         <f>S41</f>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="U41" s="15">
         <f t="shared" ref="U41:AH41" si="5">T41</f>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="V41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="W41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="X41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="Y41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="Z41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AA41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AB41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AC41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AD41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AE41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AF41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AG41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
       <c r="AH41" s="15">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>18.999999999999773</v>
       </c>
     </row>
     <row r="42" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -15556,95 +15557,95 @@
       </c>
       <c r="J112" s="18">
         <f t="shared" si="10"/>
-        <v>6.305660112124406E-2</v>
+        <v>8.7064541926442349E-2</v>
       </c>
       <c r="K112" s="18">
         <f t="shared" si="10"/>
-        <v>6.9590929459826964E-2</v>
+        <v>0.11705880094392404</v>
       </c>
       <c r="L112" s="18">
         <f t="shared" si="10"/>
-        <v>7.7086053221409809E-2</v>
+        <v>0.14851127749752255</v>
       </c>
       <c r="M112" s="18">
         <f t="shared" si="10"/>
-        <v>8.4788272018669314E-2</v>
+        <v>0.18050218542991664</v>
       </c>
       <c r="N112" s="18">
         <f t="shared" si="10"/>
-        <v>9.1642526929346116E-2</v>
+        <v>0.2106884008874772</v>
       </c>
       <c r="O112" s="18">
         <f t="shared" si="10"/>
-        <v>9.8643449064837241E-2</v>
+        <v>0.24109980506566731</v>
       </c>
       <c r="P112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10474738440532255</v>
+        <v>0.26913734538202028</v>
       </c>
       <c r="Q112" s="18">
         <f t="shared" si="10"/>
-        <v>0.11155887905676753</v>
+        <v>0.29881842604490821</v>
       </c>
       <c r="R112" s="18">
         <f t="shared" si="10"/>
-        <v>0.11027775042200511</v>
+        <v>0.29538683148750888</v>
       </c>
       <c r="S112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10921506763073226</v>
+        <v>0.29254035972517095</v>
       </c>
       <c r="T112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10908558214442861</v>
+        <v>0.29219352360114331</v>
       </c>
       <c r="U112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10815710294166644</v>
+        <v>0.28970652573660183</v>
       </c>
       <c r="V112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10841179763990781</v>
+        <v>0.29038874367831979</v>
       </c>
       <c r="W112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10802385125586841</v>
+        <v>0.28934960157821427</v>
       </c>
       <c r="X112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10779498743445363</v>
+        <v>0.28873657348513898</v>
       </c>
       <c r="Y112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10772121961190965</v>
+        <v>0.28853898110332477</v>
       </c>
       <c r="Z112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10722131825715996</v>
+        <v>0.28719995961738809</v>
       </c>
       <c r="AA112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10682428245670875</v>
+        <v>0.28613647086617949</v>
       </c>
       <c r="AB112" s="18">
         <f t="shared" si="10"/>
-        <v>0.1074216424204566</v>
+        <v>0.28773654219764694</v>
       </c>
       <c r="AC112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10706666229228147</v>
+        <v>0.28678570256860642</v>
       </c>
       <c r="AD112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10672992112007187</v>
+        <v>0.28588371728590217</v>
       </c>
       <c r="AE112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10677382613953007</v>
+        <v>0.28600132001659379</v>
       </c>
       <c r="AF112" s="18">
         <f t="shared" si="10"/>
-        <v>0.10580769668864136</v>
+        <v>0.28341347327314187</v>
       </c>
     </row>
     <row r="113" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -15681,99 +15682,99 @@
       </c>
       <c r="I113" s="18">
         <f t="shared" si="10"/>
-        <v>5.1353109362302647E-2</v>
+        <v>5.1353109362300677E-2</v>
       </c>
       <c r="J113" s="18">
         <f t="shared" si="10"/>
-        <v>7.9093467852570751E-2</v>
+        <v>5.413614667720483E-2</v>
       </c>
       <c r="K113" s="18">
         <f t="shared" si="10"/>
-        <v>0.10587163526180934</v>
+        <v>5.6871469261761405E-2</v>
       </c>
       <c r="L113" s="18">
         <f t="shared" si="10"/>
-        <v>0.13120047316016237</v>
+        <v>5.9288843556340676E-2</v>
       </c>
       <c r="M113" s="18">
         <f t="shared" si="10"/>
-        <v>0.1553034029423305</v>
+        <v>6.1542838545548761E-2</v>
       </c>
       <c r="N113" s="18">
         <f t="shared" si="10"/>
-        <v>0.17811970888717182</v>
+        <v>6.3612441513390683E-2</v>
       </c>
       <c r="O113" s="18">
         <f t="shared" si="10"/>
-        <v>0.19987053989390122</v>
+        <v>6.557582402523271E-2</v>
       </c>
       <c r="P113" s="18">
         <f t="shared" si="10"/>
-        <v>0.21916693670968349</v>
+        <v>6.6996582847732231E-2</v>
       </c>
       <c r="Q113" s="18">
         <f t="shared" si="10"/>
-        <v>0.23703309978689469</v>
+        <v>6.8236801453802204E-2</v>
       </c>
       <c r="R113" s="18">
         <f t="shared" si="10"/>
-        <v>0.23010973064913401</v>
+        <v>6.6243710338386275E-2</v>
       </c>
       <c r="S113" s="18">
         <f t="shared" si="10"/>
-        <v>0.22656075152920011</v>
+        <v>6.5222034531132594E-2</v>
       </c>
       <c r="T113" s="18">
         <f t="shared" si="10"/>
-        <v>0.22341180962001911</v>
+        <v>6.4315520951216856E-2</v>
       </c>
       <c r="U113" s="18">
         <f t="shared" si="10"/>
-        <v>0.22060889378337575</v>
+        <v>6.3508620937637719E-2</v>
       </c>
       <c r="V113" s="18">
         <f t="shared" si="10"/>
-        <v>0.21796225705452099</v>
+        <v>6.2746710364179545E-2</v>
       </c>
       <c r="W113" s="18">
         <f t="shared" si="10"/>
-        <v>0.21545696352270516</v>
+        <v>6.2025489498959835E-2</v>
       </c>
       <c r="X113" s="18">
         <f t="shared" si="10"/>
-        <v>0.21275643621905999</v>
+        <v>6.1248064972152905E-2</v>
       </c>
       <c r="Y113" s="18">
         <f t="shared" si="10"/>
-        <v>0.20902556556854876</v>
+        <v>6.0174026451551198E-2</v>
       </c>
       <c r="Z113" s="18">
         <f t="shared" si="10"/>
-        <v>0.20558434359348723</v>
+        <v>5.9183371640548647E-2</v>
       </c>
       <c r="AA113" s="18">
         <f t="shared" si="10"/>
-        <v>0.20152259911219586</v>
+        <v>5.8014081562601148E-2</v>
       </c>
       <c r="AB113" s="18">
         <f t="shared" si="10"/>
-        <v>0.19850165477144999</v>
+        <v>5.7144415767537954E-2</v>
       </c>
       <c r="AC113" s="18">
         <f t="shared" si="10"/>
-        <v>0.19586944635444359</v>
+        <v>5.6386658799005812E-2</v>
       </c>
       <c r="AD113" s="18">
         <f t="shared" si="10"/>
-        <v>0.19295510334396135</v>
+        <v>5.5547681265685184E-2</v>
       </c>
       <c r="AE113" s="18">
         <f t="shared" si="10"/>
-        <v>0.18919433415943607</v>
+        <v>5.4465035591352157E-2</v>
       </c>
       <c r="AF113" s="18">
         <f t="shared" si="10"/>
-        <v>0.18560515904050501</v>
+        <v>5.3431788208629594E-2</v>
       </c>
     </row>
     <row r="114" spans="1:32" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -21559,95 +21560,95 @@
       </c>
       <c r="J10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>5.5046192798270638E-2</v>
+        <v>7.6004279893884474E-2</v>
       </c>
       <c r="K10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>6.0750431389266571E-2</v>
+        <v>0.10218821203356511</v>
       </c>
       <c r="L10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>6.7293410558627309E-2</v>
+        <v>0.12964511674404075</v>
       </c>
       <c r="M10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>7.4017176403113505E-2</v>
+        <v>0.15757205309210551</v>
       </c>
       <c r="N10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>8.0000699628162406E-2</v>
+        <v>0.18392355644592651</v>
       </c>
       <c r="O10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>8.6112258176884934E-2</v>
+        <v>0.21047164162482773</v>
       </c>
       <c r="P10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.1440778833024969E-2</v>
+        <v>0.23494742722696807</v>
       </c>
       <c r="Q10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.7386973857188877E-2</v>
+        <v>0.26085796568889458</v>
       </c>
       <c r="R10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.6268593662656651E-2</v>
+        <v>0.25786230445354041</v>
       </c>
       <c r="S10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.5340908998852253E-2</v>
+        <v>0.25537743481835012</v>
       </c>
       <c r="T10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.5227872727995475E-2</v>
+        <v>0.25507465909284088</v>
       </c>
       <c r="U10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.4417343072168342E-2</v>
+        <v>0.25290359751473251</v>
       </c>
       <c r="V10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.4639682576911618E-2</v>
+        <v>0.2534991497595806</v>
       </c>
       <c r="W10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.4301019041746384E-2</v>
+        <v>0.25259201529038799</v>
       </c>
       <c r="X10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.4101228983066817E-2</v>
+        <v>0.25205686334749633</v>
       </c>
       <c r="Y10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.4036832271067447E-2</v>
+        <v>0.25188437215464088</v>
       </c>
       <c r="Z10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.3600435987976349E-2</v>
+        <v>0.25071545353921831</v>
       </c>
       <c r="AA10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.3253837712287027E-2</v>
+        <v>0.24978706530076475</v>
       </c>
       <c r="AB10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.3775311929890456E-2</v>
+        <v>0.2511838712407739</v>
       </c>
       <c r="AC10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.346542677547956E-2</v>
+        <v>0.25035382172003046</v>
       </c>
       <c r="AD10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.3171463587503028E-2</v>
+        <v>0.24956642032366477</v>
       </c>
       <c r="AE10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.3209791123763042E-2</v>
+        <v>0.24966908336721841</v>
       </c>
       <c r="AF10" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A10,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.2366394126841972E-2</v>
+        <v>0.24740998426832267</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -21684,99 +21685,99 @@
       </c>
       <c r="I11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!I$112:I$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>4.4829456527678731E-2</v>
+        <v>4.482945652767701E-2</v>
       </c>
       <c r="J11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!J$112:J$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>6.9045812858276892E-2</v>
+        <v>4.7258950123540727E-2</v>
       </c>
       <c r="K11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!K$112:K$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>9.2422210250186196E-2</v>
+        <v>4.9646790439663281E-2</v>
       </c>
       <c r="L11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!L$112:L$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.11453339400441416</v>
+        <v>5.1757073092372943E-2</v>
       </c>
       <c r="M11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!M$112:M$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.13557440313272587</v>
+        <v>5.3724731363450975E-2</v>
       </c>
       <c r="N11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!N$112:N$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.15549223494813161</v>
+        <v>5.5531421891610734E-2</v>
       </c>
       <c r="O11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!O$112:O$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.17447994465384317</v>
+        <v>5.7245385701296593E-2</v>
       </c>
       <c r="P11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!P$112:P$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.19132501972205246</v>
+        <v>5.8485658133881041E-2</v>
       </c>
       <c r="Q11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Q$112:Q$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.20692155108952223</v>
+        <v>5.9568325313649632E-2</v>
       </c>
       <c r="R11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!R$112:R$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.2008776935774754</v>
+        <v>5.7828426938969509E-2</v>
       </c>
       <c r="S11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!S$112:S$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.19777955975168787</v>
+        <v>5.6936539928515537E-2</v>
       </c>
       <c r="T11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!T$112:T$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.19503064432711492</v>
+        <v>5.6145185488108172E-2</v>
       </c>
       <c r="U11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!U$112:U$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.19258379748161925</v>
+        <v>5.5440790184101849E-2</v>
       </c>
       <c r="V11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!V$112:V$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.19027337679523623</v>
+        <v>5.4775669077415844E-2</v>
       </c>
       <c r="W11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!W$112:W$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.18808634374371749</v>
+        <v>5.4146068653493785E-2</v>
       </c>
       <c r="X11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!X$112:X$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.18572887848282249</v>
+        <v>5.3467404411720987E-2</v>
       </c>
       <c r="Y11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Y$112:Y$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.18247195975454267</v>
+        <v>5.2529806596004078E-2</v>
       </c>
       <c r="Z11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!Z$112:Z$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.17946789412251379</v>
+        <v>5.166499982314729E-2</v>
       </c>
       <c r="AA11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AA$112:AA$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.17592213418875879</v>
+        <v>5.0644250751308753E-2</v>
       </c>
       <c r="AB11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AB$112:AB$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.17328495613512729</v>
+        <v>4.9885063129808775E-2</v>
       </c>
       <c r="AC11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AC$112:AC$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.1709871308570225</v>
+        <v>4.9223567973990738E-2</v>
       </c>
       <c r="AD11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AD$112:AD$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.16844301201168799</v>
+        <v>4.8491170124576273E-2</v>
       </c>
       <c r="AE11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AE$112:AE$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.16515999291582636</v>
+        <v>4.7546058566676722E-2</v>
       </c>
       <c r="AF11" s="59">
         <f>IFERROR(INDEX('BAU Calculations'!AF$112:AF$115,MATCH($A11,'BAU Calculations'!$A$112:$A$115,0)),0)*'Capacity Factor Data'!$A$45</f>
-        <v>0.16202676939806096</v>
+        <v>4.6644069978229112E-2</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">

</xml_diff>